<commit_message>
ported previous IAR project
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29098" uniqueCount="236">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -147,6 +147,582 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPOGRAPHY NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll lis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll list item#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll list item#&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll list item#&lt;val&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll list item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text1&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text1&lt;value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text1&lt;value&gt;&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;tex&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Name&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;z&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;zoneName&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;v&gt;:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;val&gt;:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hour&gt;:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hour&gt;:&lt;minute&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hrf&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hF&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Tex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;dow&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABCDEFGHIJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ01234567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window Setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scene&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sceneName&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkerboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometric Patt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometric Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Go Na"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Go Navy" T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Go Navy" Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sine Wave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Che</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Tint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M Tint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual Tint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preset Scenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel Settin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesdayб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday, Ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday, May 8'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday, May 8'th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel Bri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel Brightness:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch_touchgfx/EWARM/switch_touchgfx.ewp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lee:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leep After:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eep After:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seep After:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fifteen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software v1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software v10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software v0.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP: 192.168.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP: 192.168.9.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual Style:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep After:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban</t>
   </si>
 </sst>
 </file>
@@ -1383,9 +1959,15 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
       <c r="I4"/>
       <c r="K4" s="5" t="s">
         <v>17</v>
@@ -1416,9 +1998,15 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
       <c r="I5"/>
       <c r="K5" s="8" t="s">
         <v>1</v>
@@ -1447,9 +2035,15 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
       <c r="I6"/>
       <c r="K6" s="8" t="s">
         <v>2</v>
@@ -1466,6 +2060,28 @@
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7"/>
       <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1483,6 +2099,28 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -1596,64 +2234,617 @@
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1"/>
-    <row r="5" spans="2:10" ht="15" customHeight="1"/>
-    <row r="6" spans="2:10"/>
-    <row r="7" spans="2:10"/>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
-    <row r="10" spans="2:10"/>
-    <row r="13" spans="2:10"/>
-    <row r="14" spans="2:10"/>
-    <row r="15" spans="2:10"/>
-    <row r="16" spans="2:10"/>
-    <row r="17" spans="4:4"/>
-    <row r="18" spans="4:4"/>
-    <row r="19" spans="4:4"/>
-    <row r="20" spans="4:4"/>
-    <row r="21" spans="4:4"/>
-    <row r="22" spans="4:4"/>
-    <row r="23" spans="4:4"/>
-    <row r="24" spans="4:4"/>
-    <row r="25" spans="4:4"/>
-    <row r="26" spans="4:4"/>
-    <row r="27" spans="4:4"/>
-    <row r="28" spans="4:4"/>
-    <row r="29" spans="4:4"/>
-    <row r="30" spans="4:4"/>
-    <row r="31" spans="4:4"/>
-    <row r="32" spans="4:4"/>
-    <row r="33" spans="4:4"/>
-    <row r="34" spans="4:4"/>
-    <row r="35" spans="4:4"/>
-    <row r="36" spans="4:4"/>
-    <row r="37" spans="4:4"/>
-    <row r="38" spans="4:4"/>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="B17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="B19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="B22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="B24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="B26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>195</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="B27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="B29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="B30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="B32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="B33" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="B34" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" t="s">
+        <v>222</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="B35" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>225</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" t="s">
+        <v>229</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="B37" t="s">
+        <v>230</v>
+      </c>
+      <c r="C37" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="B38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C38" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" t="s">
+        <v>235</v>
+      </c>
+      <c r="F38" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="39" spans="4:4"/>
     <row r="40" spans="4:4"/>
     <row r="41" spans="4:4"/>

</xml_diff>

<commit_message>
fixed TouchGFX bug with include directories
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29098" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29338" uniqueCount="236">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2312,7 +2312,7 @@
         <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
implemented incomint request of clock settings
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29338" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29578" uniqueCount="237">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t xml:space="preserve">Urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday, May 8th</t>
   </si>
 </sst>
 </file>
@@ -2397,7 +2400,7 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
       <c r="F12" t="s">
         <v>50</v>

</xml_diff>